<commit_message>
saving all images and gui updates
finding background index more stable
now need to move bc to inside class
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="5112" windowHeight="8712"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="5115" windowHeight="8715"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>field</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>stop</t>
+  </si>
+  <si>
+    <t>destinationfolder entry</t>
+  </si>
+  <si>
+    <t>chose destubatuibfolder button</t>
   </si>
 </sst>
 </file>
@@ -476,18 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F8" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="4.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -501,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -516,7 +524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -528,7 +536,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -543,7 +551,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -556,7 +564,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -569,7 +577,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -584,7 +592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -593,7 +601,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -604,29 +612,52 @@
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1"/>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fieldname change for new basler camera
added dialog boxes for choosing nodefile and save folder
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="5115" windowHeight="8715"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="5115" windowHeight="5610"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>field</t>
   </si>
@@ -88,7 +88,13 @@
     <t>destinationfolder entry</t>
   </si>
   <si>
-    <t>chose destubatuibfolder button</t>
+    <t>chose nodemap  button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nodemap entry </t>
+  </si>
+  <si>
+    <t>motorname</t>
   </si>
 </sst>
 </file>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F7:F8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,39 +631,63 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1"/>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>